<commit_message>
update characters moving and falling
</commit_message>
<xml_diff>
--- a/documentatie/tijdtabel.xlsx
+++ b/documentatie/tijdtabel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projecten\GIP\GIP_LS_2025\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3D1812-F02D-4908-8957-33E009F06A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BF971-9D01-410D-B340-FBC4ED5AECCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05ED82E6-A217-4E81-A4A5-6C754E771FA3}"/>
   </bookViews>
@@ -156,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +181,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -229,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -244,6 +250,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -262,9 +269,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -302,7 +309,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -408,7 +415,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,7 +568,7 @@
   <dimension ref="A1:X89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -896,8 +903,10 @@
         <f>DATE(2025,2,7)</f>
         <v>45695</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>

</xml_diff>